<commit_message>
validated string in excel
</commit_message>
<xml_diff>
--- a/platform/TestData/ValidationStrings.xlsx
+++ b/platform/TestData/ValidationStrings.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Create Account" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M9"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Label</t>
   </si>
@@ -34,6 +34,15 @@
   </si>
   <si>
     <t>パスワードの変更が完了しました。</t>
+  </si>
+  <si>
+    <t>//p[@class='alert__des']</t>
+  </si>
+  <si>
+    <t>メールアドレスは、メールアドレス形式で入力してください。</t>
+  </si>
+  <si>
+    <t>InvalidEmailError</t>
   </si>
 </sst>
 </file>
@@ -384,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -416,6 +425,17 @@
       </c>
       <c r="C2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>